<commit_message>
Agrega explicacion a Tarea 2.
</commit_message>
<xml_diff>
--- a/data_enunciado_tarea_2.xlsx
+++ b/data_enunciado_tarea_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodiaz/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB785E7-8E42-634B-A38F-B2E27B7B55C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948A7666-4D2A-B241-A367-6E5B660E1F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3140" yWindow="2000" windowWidth="27700" windowHeight="16940" xr2:uid="{6397AFD0-E58E-184D-8F61-46D23894BCF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Maturity</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Se entrega un Jupyter Notebook con la solución.</t>
+  </si>
+  <si>
+    <t>Los Caps tienen periodicidad trimestral.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,6 +516,9 @@
       <c r="D4" s="3">
         <v>1.059E-3</v>
       </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -527,12 +533,6 @@
       <c r="D5" s="3">
         <v>1.859E-3</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -547,8 +547,11 @@
       <c r="D6" s="3">
         <v>2.8869999999999998E-3</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -565,7 +568,7 @@
         <v>4.1570000000000001E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -580,6 +583,9 @@
       </c>
       <c r="D8" s="3">
         <v>5.6620000000000004E-3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>